<commit_message>
some small bug fixes for the two new attacks
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nemo/Desktop/thesis/softRmax-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F0F427-A3DF-E14A-8C9E-26DE38A83986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B5FB77-AB75-E746-8CB6-20556CC669F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21560" yWindow="4820" windowWidth="23720" windowHeight="20220" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
+    <workbookView xWindow="25340" yWindow="1400" windowWidth="23720" windowHeight="20220" activeTab="3" xr2:uid="{7CDF230F-D82A-4F4E-AAA9-9338F0541A49}"/>
   </bookViews>
   <sheets>
     <sheet name="mnist " sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="90">
   <si>
     <t xml:space="preserve">conservative_a: </t>
   </si>
@@ -294,6 +294,21 @@
   </si>
   <si>
     <t>50 samples</t>
+  </si>
+  <si>
+    <t>500 samples</t>
+  </si>
+  <si>
+    <t>Robustness (MSE)</t>
+  </si>
+  <si>
+    <t>417 samples</t>
+  </si>
+  <si>
+    <t>432 samples</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -302,8 +317,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[Colour10]0.00%;[Red]0.00%"/>
-    <numFmt numFmtId="166" formatCode="[Colour10]0%;[Red]0%"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="[Colour10]0%;[Red]0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -556,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -730,7 +745,7 @@
     <xf numFmtId="10" fontId="26" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,42 +806,24 @@
     <xf numFmtId="10" fontId="11" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,11 +831,25 @@
     </xf>
     <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A11AE0-B146-4F40-BD5E-14A3A0645060}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView topLeftCell="A4" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1754,6 +1765,23 @@
       <c r="L27" s="17"/>
       <c r="M27" s="41"/>
     </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H28" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="60">
+        <f>AVERAGE(I18:I27)</f>
+        <v>0.79966999999999988</v>
+      </c>
+      <c r="J28" s="60">
+        <f>AVERAGE(J18:J27)</f>
+        <v>0.78066000000000002</v>
+      </c>
+      <c r="K28" s="91">
+        <f>(J28-I28)/I28</f>
+        <v>-2.3772306076256286E-2</v>
+      </c>
+    </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="24"/>
       <c r="B29" s="24"/>
@@ -1773,6 +1801,9 @@
       <c r="F30" s="16"/>
       <c r="H30" s="11" t="s">
         <v>61</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="40" x14ac:dyDescent="0.25">
@@ -2143,18 +2174,18 @@
         <v>23</v>
       </c>
       <c r="B46" s="37">
-        <v>0.90090000000000003</v>
+        <v>0.92349999999999999</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="27" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="37">
-        <v>0.99165999999999999</v>
+        <v>0.90839999999999999</v>
       </c>
       <c r="F46" s="41">
         <f>(E46-B46)/B46</f>
-        <v>0.10074370074370069</v>
+        <v>-1.6350839198700597E-2</v>
       </c>
       <c r="G46" s="92"/>
       <c r="H46" s="59" t="s">
@@ -2178,31 +2209,31 @@
         <v>25</v>
       </c>
       <c r="B47" s="37">
-        <v>0.77039999999999997</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="19" t="s">
         <v>25</v>
       </c>
       <c r="E47" s="26">
-        <v>0.96516000000000002</v>
+        <v>0.80120000000000002</v>
       </c>
       <c r="F47" s="41">
         <f>(E47-B47)/B47</f>
-        <v>0.2528037383177571</v>
+        <v>-3.9328537170263717E-2</v>
       </c>
       <c r="G47" s="92"/>
       <c r="H47" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="I47" s="141">
+        <v>86</v>
+      </c>
+      <c r="I47" s="129">
         <v>4.3699999999999998E-3</v>
       </c>
-      <c r="J47" s="141">
+      <c r="J47" s="129">
         <v>1.252E-2</v>
       </c>
       <c r="K47" s="41">
-        <f t="shared" ref="K47" si="3">(J47-I47)/I47</f>
+        <f>(J47-I47)/I47</f>
         <v>1.8649885583524031</v>
       </c>
       <c r="L47" s="21"/>
@@ -2213,18 +2244,18 @@
         <v>27</v>
       </c>
       <c r="B48" s="37">
-        <v>0.58679999999999999</v>
+        <v>0.71060000000000001</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="37">
-        <v>0.90922000000000003</v>
+        <v>0.66369999999999996</v>
       </c>
       <c r="F48" s="41">
         <f>(E48-B48)/B48</f>
-        <v>0.54945466939331977</v>
+        <v>-6.6000562904587751E-2</v>
       </c>
       <c r="G48" s="92"/>
       <c r="H48" s="5" t="s">
@@ -2248,24 +2279,24 @@
         <v>29</v>
       </c>
       <c r="B49" s="37">
-        <v>0.39739999999999998</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="19" t="s">
         <v>29</v>
       </c>
       <c r="E49" s="26">
-        <v>0.78263000000000005</v>
+        <v>0.50929999999999997</v>
       </c>
       <c r="F49" s="41">
         <f>(E49-B49)/B49</f>
-        <v>0.96937594363361879</v>
+        <v>-3.7240075614366826E-2</v>
       </c>
       <c r="G49" s="92"/>
       <c r="H49" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I49" s="143">
+      <c r="I49" s="131">
         <v>4.601</v>
       </c>
       <c r="J49" s="5">
@@ -2280,18 +2311,18 @@
         <v>31</v>
       </c>
       <c r="B50" s="26">
-        <v>0.21920000000000001</v>
+        <v>0.35339999999999999</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="19" t="s">
         <v>31</v>
       </c>
       <c r="E50" s="21">
-        <v>0.59421000000000002</v>
+        <v>0.37869999999999998</v>
       </c>
       <c r="F50" s="41">
         <f>(E50-B50)/B50</f>
-        <v>1.7108120437956205</v>
+        <v>7.1590265987549487E-2</v>
       </c>
       <c r="G50" s="92"/>
       <c r="K50" s="19"/>
@@ -2307,70 +2338,50 @@
       <c r="G52" s="92"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G53" s="133"/>
-      <c r="H53" s="127"/>
-      <c r="I53" s="127"/>
-      <c r="J53" s="127"/>
-      <c r="K53" s="127"/>
-      <c r="L53" s="133"/>
+      <c r="G53" s="92"/>
+      <c r="L53" s="92"/>
       <c r="M53" s="92"/>
     </row>
     <row r="54" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="G54" s="134"/>
-      <c r="H54" s="127"/>
-      <c r="I54" s="127"/>
-      <c r="J54" s="127"/>
-      <c r="K54" s="127"/>
+      <c r="G54" s="97"/>
       <c r="L54" s="105"/>
       <c r="M54" s="106"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G55" s="133"/>
-      <c r="H55" s="127"/>
-      <c r="I55" s="127"/>
-      <c r="J55" s="127"/>
-      <c r="K55" s="127"/>
-      <c r="L55" s="144"/>
+      <c r="G55" s="92"/>
+      <c r="L55" s="107"/>
     </row>
     <row r="56" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="G56" s="133"/>
-      <c r="H56" s="122"/>
-      <c r="I56" s="127"/>
-      <c r="J56" s="127"/>
-      <c r="K56" s="127"/>
-      <c r="L56" s="144"/>
+      <c r="G56" s="92"/>
+      <c r="H56" s="11"/>
+      <c r="L56" s="107"/>
     </row>
     <row r="57" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="G57" s="133"/>
-      <c r="H57" s="127"/>
+      <c r="G57" s="92"/>
       <c r="I57" s="54"/>
       <c r="J57" s="54"/>
-      <c r="K57" s="140"/>
-      <c r="L57" s="144"/>
+      <c r="K57" s="128"/>
+      <c r="L57" s="107"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G58" s="133"/>
-      <c r="H58" s="137"/>
-      <c r="I58" s="137"/>
-      <c r="J58" s="137"/>
+      <c r="G58" s="92"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
       <c r="K58" s="41"/>
-      <c r="L58" s="144"/>
+      <c r="L58" s="107"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G59" s="133"/>
-      <c r="H59" s="137"/>
-      <c r="I59" s="145"/>
-      <c r="J59" s="145"/>
+      <c r="G59" s="92"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="129"/>
+      <c r="J59" s="129"/>
       <c r="K59" s="41"/>
-      <c r="L59" s="146"/>
+      <c r="L59" s="108"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G60" s="133"/>
-      <c r="H60" s="127"/>
-      <c r="I60" s="127"/>
-      <c r="J60" s="127"/>
+      <c r="G60" s="92"/>
       <c r="K60" s="41"/>
-      <c r="L60" s="127"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="93"/>
@@ -2379,12 +2390,8 @@
       <c r="D61" s="93"/>
       <c r="E61" s="107"/>
       <c r="F61" s="91"/>
-      <c r="G61" s="133"/>
-      <c r="H61" s="127"/>
-      <c r="I61" s="127"/>
-      <c r="J61" s="127"/>
+      <c r="G61" s="92"/>
       <c r="K61" s="41"/>
-      <c r="L61" s="127"/>
     </row>
     <row r="62" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
@@ -2393,12 +2400,7 @@
       <c r="D62" s="92"/>
       <c r="E62" s="92"/>
       <c r="F62" s="92"/>
-      <c r="G62" s="133"/>
-      <c r="H62" s="127"/>
-      <c r="I62" s="127"/>
-      <c r="J62" s="127"/>
-      <c r="K62" s="127"/>
-      <c r="L62" s="127"/>
+      <c r="G62" s="92"/>
     </row>
     <row r="63" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="115"/>
@@ -2647,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477B086D-4A69-674E-A1F5-47C7ABBEF27F}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3663,10 +3665,10 @@
       <c r="H47" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="I47" s="141">
+      <c r="I47" s="129">
         <v>6.5199999999999998E-3</v>
       </c>
-      <c r="J47" s="141">
+      <c r="J47" s="129">
         <v>3.3700000000000002E-3</v>
       </c>
       <c r="K47" s="41">
@@ -3688,11 +3690,11 @@
         <v>27</v>
       </c>
       <c r="E48" s="37">
-        <v>0.90922000000000003</v>
+        <v>0.91910000000000003</v>
       </c>
       <c r="F48" s="41">
         <f>(E48-B48)/B48</f>
-        <v>-4.6819306411707895E-2</v>
+        <v>-3.6461609426762194E-2</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>80</v>
@@ -3722,19 +3724,19 @@
         <v>29</v>
       </c>
       <c r="E49" s="26">
-        <v>0.78263000000000005</v>
+        <v>0.81210000000000004</v>
       </c>
       <c r="F49" s="41">
         <f>(E49-B49)/B49</f>
-        <v>-0.11976020964785</v>
+        <v>-8.6614704592232583E-2</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I49" s="143">
+      <c r="I49" s="131">
         <v>4.601</v>
       </c>
-      <c r="J49" s="143">
+      <c r="J49" s="131">
         <v>4.8440000000000003</v>
       </c>
       <c r="K49" s="41"/>
@@ -3753,11 +3755,11 @@
         <v>31</v>
       </c>
       <c r="E50" s="37">
-        <v>0.59421000000000002</v>
+        <v>0.67320000000000002</v>
       </c>
       <c r="F50" s="41">
         <f>(E50-B50)/B50</f>
-        <v>-0.1877938764352105</v>
+        <v>-7.9825041006014216E-2</v>
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="21"/>
@@ -4062,10 +4064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA7FE25-5858-4B4A-8ADD-8E8DDF528A8E}">
-  <dimension ref="A1:M77"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+      <selection activeCell="K26" sqref="H26:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4076,7 +4078,7 @@
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="17" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" style="5" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="16" style="5" customWidth="1"/>
@@ -4100,8 +4102,8 @@
       <c r="F2" s="10"/>
       <c r="G2" s="5"/>
       <c r="H2" s="102"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -4110,8 +4112,8 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="11"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="122"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:13" s="46" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
@@ -4134,8 +4136,8 @@
       <c r="I4" s="56"/>
       <c r="J4" s="55"/>
       <c r="K4" s="54"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="124"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="121"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4151,8 +4153,8 @@
         <v>10</v>
       </c>
       <c r="I5" s="8"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="127"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4168,8 +4170,8 @@
         <v>256</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="127"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4185,8 +4187,8 @@
         <v>15</v>
       </c>
       <c r="I7" s="8"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="127"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -4202,8 +4204,8 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I8" s="8"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="127"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4218,9 +4220,9 @@
       <c r="E9" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="I9" s="138"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="127"/>
+      <c r="I9" s="126"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4235,14 +4237,13 @@
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="139"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I11" s="8"/>
-      <c r="L11" s="125"/>
-      <c r="M11" s="127"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
@@ -4263,7 +4264,7 @@
         <v>-6.8019233024510699E-3</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="L12" s="129"/>
+      <c r="L12" s="122"/>
       <c r="M12" s="41"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -4273,7 +4274,7 @@
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
       <c r="L13" s="112"/>
-      <c r="M13" s="127"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
@@ -4341,11 +4342,15 @@
       <c r="H16" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="91" t="e">
-        <f t="shared" ref="K16:K25" si="0">(J16-I16)/I16</f>
-        <v>#DIV/0!</v>
+      <c r="I16" s="95">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="J16" s="95">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="K16" s="91">
+        <f>(J16-I16)/I16</f>
+        <v>-0.12265331664580727</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -4363,17 +4368,21 @@
         <v>0.45929999999999999</v>
       </c>
       <c r="F17" s="64">
-        <f t="shared" ref="F17:F25" si="1">(E17-B17)/B17</f>
+        <f t="shared" ref="F17:F25" si="0">(E17-B17)/B17</f>
         <v>2.7463295269168024</v>
       </c>
       <c r="H17" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="95"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="I17" s="95">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="J17" s="60">
+        <v>0.84219999999999995</v>
+      </c>
+      <c r="K17" s="91">
+        <f>(J17-I17)/I17</f>
+        <v>-2.6054002842255931E-3</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -4391,17 +4400,21 @@
         <v>0.42220000000000002</v>
       </c>
       <c r="F18" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.609170305676856</v>
       </c>
       <c r="H18" s="113" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="95"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="I18" s="95">
+        <v>0.67110000000000003</v>
+      </c>
+      <c r="J18" s="95">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="K18" s="91">
+        <f>(J18-I18)/I18</f>
+        <v>-9.4322753687974992E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -4419,17 +4432,21 @@
         <v>0.3876</v>
       </c>
       <c r="F19" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.8693467336683414</v>
       </c>
       <c r="H19" s="113" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="I19" s="95">
+        <v>0.48</v>
+      </c>
+      <c r="J19" s="95">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="K19" s="91">
+        <f t="shared" ref="K19:K24" si="1">(J19-I19)/I19</f>
+        <v>-6.8749999999999367E-3</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -4447,19 +4464,23 @@
         <v>0.35780000000000001</v>
       </c>
       <c r="F20" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5521628498727735</v>
       </c>
       <c r="H20" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="112"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L20" s="130"/>
+      <c r="I20" s="112">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="J20" s="108">
+        <v>0.89439999999999997</v>
+      </c>
+      <c r="K20" s="91">
+        <f t="shared" si="1"/>
+        <v>0.17854789827381731</v>
+      </c>
+      <c r="L20" s="123"/>
       <c r="M20" s="41"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -4477,19 +4498,23 @@
         <v>0.33069999999999999</v>
       </c>
       <c r="F21" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.1755050505050502</v>
       </c>
       <c r="H21" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="129"/>
+      <c r="I21" s="60">
+        <v>0.6633</v>
+      </c>
+      <c r="J21" s="60">
+        <v>0.65780000000000005</v>
+      </c>
+      <c r="K21" s="91">
+        <f t="shared" si="1"/>
+        <v>-8.2918739635156787E-3</v>
+      </c>
+      <c r="L21" s="122"/>
       <c r="M21" s="41"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4507,19 +4532,23 @@
         <v>0.30520000000000003</v>
       </c>
       <c r="F22" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.6507177033492826</v>
       </c>
       <c r="H22" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="130"/>
+      <c r="I22" s="22">
+        <v>0.89780000000000004</v>
+      </c>
+      <c r="J22" s="60">
+        <v>0.8911</v>
+      </c>
+      <c r="K22" s="91">
+        <f t="shared" si="1"/>
+        <v>-7.4626865671642223E-3</v>
+      </c>
+      <c r="L22" s="123"/>
       <c r="M22" s="41"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4537,19 +4566,23 @@
         <v>0.28010000000000002</v>
       </c>
       <c r="F23" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.2048054919908466</v>
       </c>
       <c r="H23" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="22"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L23" s="130"/>
+      <c r="I23" s="22">
+        <v>0.84330000000000005</v>
+      </c>
+      <c r="J23" s="60">
+        <v>0.61560000000000004</v>
+      </c>
+      <c r="K23" s="91">
+        <f t="shared" si="1"/>
+        <v>-0.27001067235859127</v>
+      </c>
+      <c r="L23" s="123"/>
       <c r="M23" s="41"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4567,19 +4600,23 @@
         <v>0.26019999999999999</v>
       </c>
       <c r="F24" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8975501113585744</v>
       </c>
       <c r="H24" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="I24" s="22"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L24" s="130"/>
+      <c r="I24" s="22">
+        <v>0.84670000000000001</v>
+      </c>
+      <c r="J24" s="60">
+        <v>0.85560000000000003</v>
+      </c>
+      <c r="K24" s="91">
+        <f t="shared" si="1"/>
+        <v>1.0511397189087066E-2</v>
+      </c>
+      <c r="L24" s="123"/>
       <c r="M24" s="41"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4597,24 +4634,42 @@
         <v>0.23719999999999999</v>
       </c>
       <c r="F25" s="64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5127118644067794</v>
       </c>
       <c r="H25" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="91" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L25" s="130"/>
+      <c r="I25" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="J25" s="60">
+        <v>0.86329999999999996</v>
+      </c>
+      <c r="K25" s="91">
+        <f>(J25-I25)/I25</f>
+        <v>-4.077777777777785E-2</v>
+      </c>
+      <c r="L25" s="123"/>
       <c r="M25" s="41"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L26" s="125"/>
-      <c r="M26" s="127"/>
+      <c r="H26" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="60">
+        <f>AVERAGE(I16:I25)</f>
+        <v>0.77844000000000002</v>
+      </c>
+      <c r="J26" s="60">
+        <f>AVERAGE(J16:J25)</f>
+        <v>0.74755999999999989</v>
+      </c>
+      <c r="K26" s="91">
+        <f>(J26-I26)/I26</f>
+        <v>-3.9669081753250256E-2</v>
+      </c>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="31"/>
@@ -4623,7 +4678,7 @@
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
       <c r="L27" s="112"/>
-      <c r="M27" s="127"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -4637,8 +4692,14 @@
       <c r="H28" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="I28" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" s="137" t="s">
+        <v>87</v>
+      </c>
       <c r="L28" s="112"/>
-      <c r="M28" s="127"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" s="46" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
@@ -4690,20 +4751,18 @@
         <v>-0.46039076376554167</v>
       </c>
       <c r="H30" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="I30" s="59">
-        <v>0.01</v>
+        <v>81</v>
+      </c>
+      <c r="I30" s="132">
+        <v>1.5879999999999998E-2</v>
       </c>
       <c r="J30" s="59">
-        <v>0.16</v>
+        <v>0.26074999999999998</v>
       </c>
       <c r="K30" s="41">
         <f>(J30-I30)/I30</f>
-        <v>15</v>
-      </c>
-      <c r="L30" s="125"/>
-      <c r="M30" s="125"/>
+        <v>15.420025188916878</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
@@ -4724,16 +4783,19 @@
         <v>-0.68714401952807158</v>
       </c>
       <c r="H31" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" s="28">
-        <v>0</v>
-      </c>
-      <c r="J31" s="28">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="K31" s="41"/>
-      <c r="L31" s="130"/>
+        <v>86</v>
+      </c>
+      <c r="I31" s="133">
+        <v>5.0250000000000002E-4</v>
+      </c>
+      <c r="J31" s="129">
+        <v>0.28505540000000001</v>
+      </c>
+      <c r="K31" s="41">
+        <f t="shared" ref="K31:K34" si="3">(J31-I31)/I31</f>
+        <v>566.27442786069651</v>
+      </c>
+      <c r="L31" s="123"/>
       <c r="M31" s="41"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4755,19 +4817,16 @@
         <v>-0.75088183421516752</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I32" s="5">
-        <v>3.14</v>
-      </c>
-      <c r="J32" s="5">
-        <v>6.9379999999999997</v>
-      </c>
-      <c r="K32" s="41">
-        <f>(J32-I32)/I32</f>
-        <v>1.2095541401273884</v>
-      </c>
-      <c r="L32" s="130"/>
+        <v>62</v>
+      </c>
+      <c r="I32" s="136">
+        <v>0</v>
+      </c>
+      <c r="J32" s="24">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="K32" s="41"/>
+      <c r="L32" s="123"/>
       <c r="M32" s="41"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4789,19 +4848,19 @@
         <v>-0.76877657061880023</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I33" s="5">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="J33" s="5">
-        <v>0.58199999999999996</v>
+        <v>64</v>
+      </c>
+      <c r="I33" s="134">
+        <v>3.19</v>
+      </c>
+      <c r="J33" s="130">
+        <v>3.4359999999999999</v>
       </c>
       <c r="K33" s="41">
-        <f>(J33-I33)/I33</f>
-        <v>0.82445141065830707</v>
-      </c>
-      <c r="L33" s="130"/>
+        <f t="shared" si="3"/>
+        <v>7.711598746081505E-2</v>
+      </c>
+      <c r="L33" s="123"/>
       <c r="M33" s="41"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4822,8 +4881,21 @@
         <f t="shared" si="2"/>
         <v>-0.77103518612952582</v>
       </c>
-      <c r="L34" s="120"/>
-      <c r="M34" s="120"/>
+      <c r="H34" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="135">
+        <v>0.254</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K34" s="41">
+        <f t="shared" si="3"/>
+        <v>0.12204724409448808</v>
+      </c>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
@@ -4843,8 +4915,6 @@
         <f t="shared" si="2"/>
         <v>-0.75940054495912812</v>
       </c>
-      <c r="L35" s="125"/>
-      <c r="M35" s="125"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
@@ -4865,8 +4935,6 @@
         <v>-0.73516515638702129</v>
       </c>
       <c r="K36" s="41"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="125"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
@@ -4924,13 +4992,6 @@
         <f t="shared" si="2"/>
         <v>-0.63786008230452673</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H41" s="127"/>
-      <c r="I41" s="127"/>
-      <c r="J41" s="127"/>
-      <c r="K41" s="127"/>
-      <c r="L41" s="125"/>
     </row>
     <row r="42" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="77" t="s">
@@ -4941,11 +5002,7 @@
       <c r="D42" s="77"/>
       <c r="E42" s="78"/>
       <c r="F42" s="87"/>
-      <c r="H42" s="122"/>
-      <c r="I42" s="127"/>
-      <c r="J42" s="127"/>
-      <c r="K42" s="127"/>
-      <c r="L42" s="125"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="1:13" ht="40" x14ac:dyDescent="0.2">
       <c r="A43" s="79" t="s">
@@ -4964,11 +5021,9 @@
       <c r="F43" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="H43" s="127"/>
       <c r="I43" s="54"/>
       <c r="J43" s="54"/>
-      <c r="K43" s="140"/>
-      <c r="L43" s="125"/>
+      <c r="K43" s="128"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="72" t="s">
@@ -4985,14 +5040,13 @@
         <v>0.64039999999999997</v>
       </c>
       <c r="F44" s="86">
-        <f t="shared" ref="F44:F47" si="3">(E44-B44)/B44</f>
+        <f t="shared" ref="F44:F47" si="4">(E44-B44)/B44</f>
         <v>2.546036829463557E-2</v>
       </c>
-      <c r="H44" s="137"/>
-      <c r="I44" s="137"/>
-      <c r="J44" s="137"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
       <c r="K44" s="41"/>
-      <c r="L44" s="125"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="83" t="s">
@@ -5009,14 +5063,13 @@
         <v>0.45779999999999998</v>
       </c>
       <c r="F45" s="86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.8328358208955216</v>
       </c>
-      <c r="H45" s="137"/>
-      <c r="I45" s="145"/>
-      <c r="J45" s="145"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="129"/>
       <c r="K45" s="41"/>
-      <c r="L45" s="125"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="82" t="s">
@@ -5033,14 +5086,10 @@
         <v>0.36159999999999998</v>
       </c>
       <c r="F46" s="86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79.355555555555554</v>
       </c>
-      <c r="H46" s="127"/>
-      <c r="I46" s="127"/>
-      <c r="J46" s="127"/>
       <c r="K46" s="41"/>
-      <c r="L46" s="125"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="85" t="s">
@@ -5057,25 +5106,20 @@
         <v>0.104</v>
       </c>
       <c r="F47" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1038.9999999999998</v>
       </c>
-      <c r="H47" s="127"/>
-      <c r="I47" s="127"/>
-      <c r="J47" s="147"/>
+      <c r="J47" s="130"/>
       <c r="K47" s="41"/>
-      <c r="L47" s="125"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" s="2"/>
       <c r="F48" s="41"/>
-      <c r="H48" s="127"/>
       <c r="I48" s="21"/>
       <c r="J48" s="22"/>
       <c r="K48" s="19"/>
-      <c r="L48" s="125"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="2"/>
       <c r="F49" s="41"/>
@@ -5083,170 +5127,161 @@
       <c r="I49" s="21"/>
       <c r="J49" s="22"/>
       <c r="K49" s="19"/>
-      <c r="L49" s="125"/>
-    </row>
-    <row r="50" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
-      <c r="B50" s="132"/>
-      <c r="C50" s="133"/>
-      <c r="D50" s="133"/>
-      <c r="E50" s="133"/>
-      <c r="F50" s="133"/>
+      <c r="B50" s="124"/>
+      <c r="C50" s="92"/>
+      <c r="D50" s="92"/>
+      <c r="E50" s="92"/>
+      <c r="F50" s="92"/>
       <c r="H50" s="19"/>
       <c r="I50" s="21"/>
       <c r="J50" s="22"/>
       <c r="K50" s="19"/>
-      <c r="L50" s="125"/>
-    </row>
-    <row r="51" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="115"/>
       <c r="B51" s="105"/>
-      <c r="C51" s="134"/>
+      <c r="C51" s="97"/>
       <c r="D51" s="105"/>
       <c r="E51" s="105"/>
       <c r="F51" s="106"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="93"/>
       <c r="B52" s="110"/>
-      <c r="C52" s="133"/>
+      <c r="C52" s="92"/>
       <c r="D52" s="93"/>
       <c r="E52" s="110"/>
       <c r="F52" s="91"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="93"/>
       <c r="B53" s="110"/>
-      <c r="C53" s="133"/>
+      <c r="C53" s="92"/>
       <c r="D53" s="93"/>
       <c r="E53" s="110"/>
       <c r="F53" s="91"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="93"/>
       <c r="B54" s="110"/>
-      <c r="C54" s="133"/>
+      <c r="C54" s="92"/>
       <c r="D54" s="93"/>
       <c r="E54" s="110"/>
       <c r="F54" s="91"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="93"/>
       <c r="B55" s="110"/>
-      <c r="C55" s="133"/>
+      <c r="C55" s="92"/>
       <c r="D55" s="93"/>
       <c r="E55" s="110"/>
       <c r="F55" s="91"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="29"/>
-      <c r="B56" s="135"/>
-      <c r="C56" s="131"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="3"/>
       <c r="D56" s="29"/>
-      <c r="E56" s="135"/>
+      <c r="E56" s="125"/>
       <c r="F56" s="91"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="93"/>
       <c r="B57" s="110"/>
-      <c r="C57" s="133"/>
+      <c r="C57" s="92"/>
       <c r="D57" s="93"/>
       <c r="E57" s="110"/>
       <c r="F57" s="91"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="93"/>
       <c r="B58" s="110"/>
-      <c r="C58" s="133"/>
+      <c r="C58" s="92"/>
       <c r="D58" s="93"/>
       <c r="E58" s="110"/>
       <c r="F58" s="91"/>
     </row>
-    <row r="59" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
-      <c r="B59" s="132"/>
-      <c r="C59" s="133"/>
-      <c r="D59" s="133"/>
-      <c r="E59" s="132"/>
-      <c r="F59" s="133"/>
-    </row>
-    <row r="60" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="B59" s="124"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="92"/>
+      <c r="E59" s="124"/>
+      <c r="F59" s="92"/>
+    </row>
+    <row r="60" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A60" s="115"/>
       <c r="B60" s="105"/>
-      <c r="C60" s="134"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="105"/>
       <c r="E60" s="105"/>
       <c r="F60" s="106"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="93"/>
       <c r="B61" s="110"/>
-      <c r="C61" s="133"/>
+      <c r="C61" s="92"/>
       <c r="D61" s="93"/>
       <c r="E61" s="110"/>
       <c r="F61" s="91"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="93"/>
       <c r="B62" s="110"/>
-      <c r="C62" s="133"/>
+      <c r="C62" s="92"/>
       <c r="D62" s="93"/>
       <c r="E62" s="110"/>
       <c r="F62" s="91"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="93"/>
       <c r="B63" s="110"/>
-      <c r="C63" s="133"/>
+      <c r="C63" s="92"/>
       <c r="D63" s="93"/>
       <c r="E63" s="110"/>
       <c r="F63" s="91"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="93"/>
       <c r="B64" s="110"/>
-      <c r="C64" s="133"/>
+      <c r="C64" s="92"/>
       <c r="D64" s="93"/>
       <c r="E64" s="110"/>
       <c r="F64" s="91"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="93"/>
-      <c r="B65" s="136"/>
-      <c r="C65" s="125"/>
+      <c r="B65" s="100"/>
       <c r="D65" s="93"/>
-      <c r="E65" s="136"/>
+      <c r="E65" s="100"/>
       <c r="F65" s="91"/>
       <c r="H65" s="111"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="125"/>
-      <c r="B66" s="126"/>
-      <c r="C66" s="125"/>
-      <c r="D66" s="125"/>
-      <c r="E66" s="126"/>
-      <c r="F66" s="137"/>
+      <c r="B66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="59"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="125"/>
-      <c r="B67" s="126"/>
-      <c r="C67" s="125"/>
-      <c r="D67" s="125"/>
-      <c r="E67" s="126"/>
-      <c r="F67" s="137"/>
+      <c r="B67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="59"/>
     </row>
     <row r="68" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="30"/>
-      <c r="B68" s="132"/>
-      <c r="C68" s="133"/>
-      <c r="D68" s="133"/>
-      <c r="E68" s="132"/>
-      <c r="F68" s="133"/>
+      <c r="B68" s="124"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="124"/>
+      <c r="F68" s="92"/>
     </row>
     <row r="69" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A69" s="115"/>
       <c r="B69" s="105"/>
-      <c r="C69" s="134"/>
+      <c r="C69" s="97"/>
       <c r="D69" s="105"/>
       <c r="E69" s="105"/>
       <c r="F69" s="106"/>
@@ -5254,7 +5289,7 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="93"/>
       <c r="B70" s="110"/>
-      <c r="C70" s="133"/>
+      <c r="C70" s="92"/>
       <c r="D70" s="93"/>
       <c r="E70" s="110"/>
       <c r="F70" s="91"/>
@@ -5262,7 +5297,7 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="93"/>
       <c r="B71" s="110"/>
-      <c r="C71" s="133"/>
+      <c r="C71" s="92"/>
       <c r="D71" s="93"/>
       <c r="E71" s="110"/>
       <c r="F71" s="91"/>
@@ -5270,7 +5305,7 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="93"/>
       <c r="B72" s="110"/>
-      <c r="C72" s="133"/>
+      <c r="C72" s="92"/>
       <c r="D72" s="93"/>
       <c r="E72" s="110"/>
       <c r="F72" s="91"/>
@@ -5278,42 +5313,17 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="93"/>
       <c r="B73" s="110"/>
-      <c r="C73" s="133"/>
+      <c r="C73" s="92"/>
       <c r="D73" s="93"/>
       <c r="E73" s="110"/>
       <c r="F73" s="91"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="93"/>
-      <c r="B74" s="136"/>
-      <c r="C74" s="125"/>
+      <c r="B74" s="100"/>
       <c r="D74" s="93"/>
-      <c r="E74" s="136"/>
+      <c r="E74" s="100"/>
       <c r="F74" s="91"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="125"/>
-      <c r="B75" s="125"/>
-      <c r="C75" s="125"/>
-      <c r="D75" s="125"/>
-      <c r="E75" s="125"/>
-      <c r="F75" s="127"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="125"/>
-      <c r="B76" s="125"/>
-      <c r="C76" s="125"/>
-      <c r="D76" s="125"/>
-      <c r="E76" s="125"/>
-      <c r="F76" s="127"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="125"/>
-      <c r="B77" s="125"/>
-      <c r="C77" s="125"/>
-      <c r="D77" s="125"/>
-      <c r="E77" s="125"/>
-      <c r="F77" s="127"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5325,8 +5335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B838E109-CF6D-004A-85D1-C7667BDB836D}">
   <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="94" workbookViewId="0">
-      <selection activeCell="K49" sqref="H44:K49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5907,6 +5917,23 @@
         <v>-0.21285448374028251</v>
       </c>
     </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="60">
+        <f>AVERAGE(I18:I27)</f>
+        <v>0.84008000000000005</v>
+      </c>
+      <c r="J28" s="60">
+        <f>AVERAGE(J18:J27)</f>
+        <v>0.65989999999999982</v>
+      </c>
+      <c r="K28" s="91">
+        <f>(J28-I28)/I28</f>
+        <v>-0.21447957337396464</v>
+      </c>
+    </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="24"/>
       <c r="B29" s="24"/>
@@ -6302,14 +6329,14 @@
       <c r="H47" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="I47" s="141">
+      <c r="I47" s="129">
         <v>2.1910000000000001E-4</v>
       </c>
-      <c r="J47" s="141">
+      <c r="J47" s="129">
         <v>2.6479999999999999E-4</v>
       </c>
       <c r="K47" s="41">
-        <f t="shared" ref="K47:K50" si="4">(J47-I47)/I47</f>
+        <f t="shared" ref="K47" si="4">(J47-I47)/I47</f>
         <v>0.20858055682336818</v>
       </c>
     </row>
@@ -6369,7 +6396,7 @@
       <c r="I49" s="5">
         <v>8.76</v>
       </c>
-      <c r="J49" s="142">
+      <c r="J49" s="130">
         <v>9.1199999999999992</v>
       </c>
       <c r="K49" s="41"/>

</xml_diff>